<commit_message>
Budget Anonymous AU test cases
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
+++ b/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Documents/untitled folder 3/ecom-us-web/budget-web-tests/testData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDFFA0C-B294-1B40-B4BB-2606D7BC8BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="22368" windowHeight="9215"/>
   </bookViews>
   <sheets>
     <sheet name="Budget US Anonymous" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="100">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -212,6 +206,12 @@
     <t>PickUplocation1</t>
   </si>
   <si>
+    <t>CreditCardType</t>
+  </si>
+  <si>
+    <t>AnonymousUserTestCases</t>
+  </si>
+  <si>
     <t>Budget_Reservation_Domestic_Anonymous_PayLater_AU</t>
   </si>
   <si>
@@ -248,10 +248,61 @@
     <t>Budget_Reservation_Outbound_PayLater_AU</t>
   </si>
   <si>
-    <t>AnonymousUserTestCases</t>
-  </si>
-  <si>
     <t>Budget_Reservation_Domestic_PayNow_AU</t>
+  </si>
+  <si>
+    <t>PayNow</t>
+  </si>
+  <si>
+    <t>342000000000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">701 West </t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>0123141G</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Inbound_PayNow_AU</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Outbound_PayNow_AU</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_TtypeCoupon_PayLater_AU</t>
+  </si>
+  <si>
+    <t>LAS</t>
+  </si>
+  <si>
+    <t>MUZZ012</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_MtypeCoupon_PayLater_AU</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_UtypeCoupon_PayLater_AU</t>
+  </si>
+  <si>
+    <t>UUZZ006</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_GtypeCoupon_PayLater_AU</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_AWDorBCD_PayLater_AU</t>
   </si>
   <si>
     <t>username</t>
@@ -269,12 +320,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,21 +358,351 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -325,50 +710,345 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -626,33 +1306,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:BL29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.8333333333333" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
-    <col min="22" max="22" width="11.1640625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1111111111111"/>
+    <col min="10" max="10" width="12.5555555555556" customWidth="1"/>
+    <col min="22" max="22" width="11.1666666666667" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.3333333333333" customWidth="1"/>
     <col min="24" max="24" width="12.5" customWidth="1"/>
-    <col min="25" max="25" width="8.6640625" customWidth="1"/>
-    <col min="33" max="33" width="13.1640625" customWidth="1"/>
-    <col min="49" max="49" width="15.33203125" customWidth="1"/>
+    <col min="25" max="25" width="8.66666666666667" customWidth="1"/>
+    <col min="33" max="33" width="13.1666666666667" customWidth="1"/>
+    <col min="49" max="49" width="15.3333333333333" customWidth="1"/>
     <col min="50" max="50" width="15.5" customWidth="1"/>
     <col min="51" max="51" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.6" spans="1:64">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +1350,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -818,16 +1500,16 @@
       <c r="BC1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="3" t="s">
         <v>58</v>
       </c>
       <c r="BH1" s="2" t="s">
@@ -839,870 +1521,2126 @@
       <c r="BJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
+    <row r="2" spans="1:64">
+      <c r="A2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="U2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V2" s="1">
         <v>9838234567</v>
       </c>
       <c r="W2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="X2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Y2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Z2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AB2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AC2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AD2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AE2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AG2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AH2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AK2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AL2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AM2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AP2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AR2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AT2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AU2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AV2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AX2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AY2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AZ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BA2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BB2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BC2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64">
+      <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" t="s">
         <v>71</v>
       </c>
-      <c r="BF2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="U3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" t="s">
-        <v>69</v>
-      </c>
-      <c r="U3" t="s">
-        <v>70</v>
       </c>
       <c r="V3" s="1">
         <v>9838234567</v>
       </c>
       <c r="W3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="X3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Y3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Z3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AC3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AD3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AG3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AH3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AK3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AL3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AM3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AP3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AR3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AT3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AU3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AV3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AX3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AY3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AZ3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BA3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BB3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BC3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64">
+      <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" t="s">
         <v>71</v>
       </c>
-      <c r="BF3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" t="s">
-        <v>69</v>
-      </c>
       <c r="U4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V4" s="1">
         <v>9838234567</v>
       </c>
       <c r="W4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="X4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Y4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Z4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AB4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AC4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AD4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AE4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AG4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AH4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AK4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AL4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AM4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AP4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AR4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AT4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AU4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AV4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AX4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AY4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AZ4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BA4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BB4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BC4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64">
+      <c r="A5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s">
+        <v>67</v>
+      </c>
+      <c r="P5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" t="s">
+        <v>78</v>
+      </c>
+      <c r="S5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" t="s">
         <v>71</v>
       </c>
-      <c r="BF4" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" t="s">
-        <v>65</v>
-      </c>
-      <c r="O5" t="s">
-        <v>65</v>
-      </c>
-      <c r="P5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" t="s">
-        <v>69</v>
-      </c>
       <c r="U5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V5" s="1">
         <v>9838234567</v>
       </c>
-      <c r="W5" t="s">
-        <v>65</v>
-      </c>
-      <c r="X5" t="s">
-        <v>65</v>
+      <c r="W5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="X5">
+        <v>1129</v>
       </c>
       <c r="Y5" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="Z5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="AA5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>65</v>
+        <v>82</v>
+      </c>
+      <c r="AB5">
+        <v>123</v>
       </c>
       <c r="AC5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AD5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="AE5">
+        <v>6000</v>
       </c>
       <c r="AF5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AG5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AH5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AK5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AL5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AM5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AP5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AR5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AT5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AU5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AV5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AX5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AY5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AZ5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BA5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BB5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC5">
+        <v>2323</v>
+      </c>
+      <c r="BD5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64">
+      <c r="A6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T6" t="s">
         <v>71</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="U6" t="s">
+        <v>72</v>
+      </c>
+      <c r="V6" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="X6">
+        <v>1129</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB6">
+        <v>123</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC6">
+        <v>2323</v>
+      </c>
+      <c r="BD6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64">
+      <c r="A7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" t="s">
         <v>71</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="U7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="V7" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="X7">
+        <v>1129</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB7">
+        <v>123</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE7">
+        <v>6000</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC7">
+        <v>2323</v>
+      </c>
+      <c r="BD7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64">
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" t="s">
+        <v>69</v>
+      </c>
+      <c r="S8" t="s">
+        <v>70</v>
+      </c>
+      <c r="T8" t="s">
         <v>71</v>
       </c>
-      <c r="BH5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>65</v>
+      <c r="U8" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W8" t="s">
+        <v>67</v>
+      </c>
+      <c r="X8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F6" s="3"/>
-      <c r="W6" s="6"/>
+    <row r="9" spans="1:64">
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S9" t="s">
+        <v>70</v>
+      </c>
+      <c r="T9" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" t="s">
+        <v>72</v>
+      </c>
+      <c r="V9" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W9" t="s">
+        <v>67</v>
+      </c>
+      <c r="X9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F7" s="3"/>
-      <c r="W7" s="6"/>
+    <row r="10" spans="1:64">
+      <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" t="s">
+        <v>93</v>
+      </c>
+      <c r="N10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" t="s">
+        <v>67</v>
+      </c>
+      <c r="P10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T10" t="s">
+        <v>71</v>
+      </c>
+      <c r="U10" t="s">
+        <v>72</v>
+      </c>
+      <c r="V10" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W10" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F8" s="3"/>
+    <row r="11" spans="1:64">
+      <c r="A11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="5">
+        <v>45090</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45100</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" t="s">
+        <v>67</v>
+      </c>
+      <c r="O11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T11" t="s">
+        <v>71</v>
+      </c>
+      <c r="U11" t="s">
+        <v>72</v>
+      </c>
+      <c r="V11" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F9" s="3"/>
+    <row r="12" spans="1:62">
+      <c r="A12" s="3"/>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="AG12" s="9"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
+      <c r="BI12" s="3"/>
+      <c r="BJ12" s="3"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F10" s="3"/>
+    <row r="13" spans="1:62">
+      <c r="A13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F11" s="3"/>
+    <row r="14" spans="1:63">
+      <c r="A14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="8"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+      <c r="BK14" s="4"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F12" s="3"/>
-      <c r="AG12" s="7"/>
+    <row r="15" spans="1:62">
+      <c r="A15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
+      <c r="BH15" s="3"/>
+      <c r="BI15" s="3"/>
+      <c r="BJ15" s="3"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F13" s="3"/>
+    <row r="16" ht="15" spans="1:62">
+      <c r="A16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="BB16" s="10"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
+      <c r="BI16" s="3"/>
+      <c r="BJ16" s="3"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="BK14" s="3"/>
+    <row r="17" spans="1:62">
+      <c r="A17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="3"/>
+      <c r="BH17" s="3"/>
+      <c r="BI17" s="3"/>
+      <c r="BJ17" s="3"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="F15" s="3"/>
-      <c r="H15" s="4"/>
+    <row r="18" spans="1:62">
+      <c r="A18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="M18" s="6"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="3"/>
+      <c r="BH18" s="3"/>
+      <c r="BI18" s="3"/>
+      <c r="BJ18" s="3"/>
     </row>
-    <row r="16" spans="1:63" ht="16" x14ac:dyDescent="0.2">
-      <c r="F16" s="3"/>
-      <c r="BB16" s="8"/>
+    <row r="19" spans="1:62">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
+      <c r="BH19" s="3"/>
+      <c r="BI19" s="3"/>
+      <c r="BJ19" s="3"/>
     </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F17" s="3"/>
+    <row r="20" spans="1:62">
+      <c r="A20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BH20" s="3"/>
+      <c r="BI20" s="3"/>
+      <c r="BJ20" s="3"/>
     </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F18" s="3"/>
-      <c r="M18" s="5"/>
+    <row r="21" spans="1:62">
+      <c r="A21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
+      <c r="BI21" s="3"/>
+      <c r="BJ21" s="3"/>
     </row>
-    <row r="19" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.2">
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="22:22">
       <c r="V22"/>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="22:22">
       <c r="V23"/>
     </row>
-    <row r="24" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="22:22">
       <c r="V24"/>
     </row>
-    <row r="25" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="22:22">
       <c r="V25"/>
     </row>
-    <row r="26" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="22:22">
       <c r="V26"/>
     </row>
-    <row r="27" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="22:22">
       <c r="V27"/>
     </row>
-    <row r="28" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="22:22">
       <c r="V28"/>
     </row>
-    <row r="29" spans="6:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="22:22">
       <c r="V29"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U7" r:id="rId1" display="automation@yopmail.com" tooltip="mailto:automation@yopmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:BA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1713,10 +3651,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1863,165 +3801,166 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:53">
       <c r="B2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="U2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="V2">
         <v>9838234567</v>
       </c>
       <c r="W2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="X2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Y2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Z2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AB2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AC2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AD2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AE2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AG2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AH2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AJ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AK2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AL2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AM2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AN2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AP2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AQ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AR2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AT2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AU2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AV2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AX2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AY2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AZ2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="BA2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Budget Test cases fixes
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
+++ b/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/Budget_Payless 27 Apr/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5015FD12-3D39-3C46-9F38-691FFAE81F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1B3FB9-39F8-3E4E-913B-2E2CD4A3EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -822,7 +822,7 @@
   <dimension ref="A1:BR29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B3" sqref="A1:BR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Budget AU Domain fixes
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
+++ b/budget-web-tests/testData/Budget_Anonymous_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/Budget_Payless 27 Apr/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD17E02F-EEFC-1849-9199-57AE5798C3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA16984D-7457-2C42-B27C-FEF7ADF677E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="119">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -402,8 +402,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -499,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -514,14 +514,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -812,7 +812,7 @@
   <dimension ref="A1:BR29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="A1:BR21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -842,7 +842,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3540,10 +3540,10 @@
         <v>73</v>
       </c>
       <c r="BB13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="BC13" s="4">
-        <v>2323</v>
+        <v>73</v>
+      </c>
+      <c r="BC13" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="BD13" s="4" t="s">
         <v>73</v>

</xml_diff>